<commit_message>
Implemented the Cart class and added new commands.
</commit_message>
<xml_diff>
--- a/GroceryCoCheckout/Data/ShoppingList.xlsx
+++ b/GroceryCoCheckout/Data/ShoppingList.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="4">
   <si>
     <t>Name</t>
   </si>
@@ -376,9 +376,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -407,6 +409,11 @@
         <v>3</v>
       </c>
     </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Fixed group pricing to apply correctly for multiple items greater than defined amount.
</commit_message>
<xml_diff>
--- a/GroceryCoCheckout/Data/ShoppingList.xlsx
+++ b/GroceryCoCheckout/Data/ShoppingList.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="6">
   <si>
     <t>Name</t>
   </si>
@@ -29,6 +29,9 @@
   </si>
   <si>
     <t>Orange</t>
+  </si>
+  <si>
+    <t>Tomato</t>
   </si>
 </sst>
 </file>
@@ -379,10 +382,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:A14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -432,6 +435,36 @@
         <v>4</v>
       </c>
     </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>